<commit_message>
Add NBs for direct data entry and recording query exection times
</commit_message>
<xml_diff>
--- a/obs.xlsx
+++ b/obs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College\Sem_4\251\Research Paper\Data-Selection-in-NoSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5770C9E-6CBD-4C52-8C3A-B0EAA15D8050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB15854-43A6-43F9-88CD-45C9672849CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -125,11 +125,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
@@ -445,103 +445,105 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1.6659999999999999E-3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2">
         <v>100000</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.23420374999999999</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1000</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>1.7825E-3</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2">
         <v>100000</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.17884725000000001</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.0177612499999995</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>1000</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>1.2615E-3</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2">
         <v>100000</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>9.0697E-2</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>